<commit_message>
change some stuf on general results
</commit_message>
<xml_diff>
--- a/src/excels/meningeal/updates/cluster_cell_counts_all.xlsx
+++ b/src/excels/meningeal/updates/cluster_cell_counts_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,21 +448,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MeV.VLMC.0</t>
+          <t>MeV.Fib.0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>345</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MeV.ECM.1</t>
+          <t>MeV.VLMC.0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>280</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
@@ -478,7 +478,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MeV.Fib.1</t>
+          <t>MeV.FibCollagen.3</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -508,7 +508,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MeV.Fib.3</t>
+          <t>MeV.Fib.2</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -518,7 +518,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MeV.Fib.2</t>
+          <t>MeV.Fib.1</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -528,7 +528,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MeV.ECM.2</t>
+          <t>MeV.FibCollagen.0</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -548,130 +548,120 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MeV.Fib.0</t>
+          <t>MeV.Endothelial.1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>176</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MeV.Endothelial.1</t>
+          <t>MeV.VLMC.1</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MeV.VLMC.1</t>
+          <t>MeV.FibLaminin.0</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MeV.ECM.0</t>
+          <t>MeV.Endothelial.3</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MeV.Endothelial.3</t>
+          <t>MeV.Fib.4</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MeV.Fib.6</t>
+          <t>MeV.Epithelial.0</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MeV.EpithelialECad.0</t>
+          <t>MeV.FibCollagen.2</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MeV.FibCD34.7</t>
+          <t>MeV.SMC.0</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MeV.SMC.0</t>
+          <t>MeV.FibCollagen.1</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MeV.Fib.4</t>
+          <t>MeV.Fib.3</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MeV.Fib.5</t>
+          <t>MeV.EndoUnknowed.4</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MeV.EndoUnknowed.4</t>
+          <t>MeV.FibProlif.0</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>MeV.FibProlif.0</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
         <v>21</v>
       </c>
     </row>

</xml_diff>